<commit_message>
add discord user verification with ids, fix admin checklist details, all that fun stuff
</commit_message>
<xml_diff>
--- a/server/utils/osrs_content_manager.xlsx
+++ b/server/utils/osrs_content_manager.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lgarrett/personal_projects/osrs-bingo/server/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE46EFB-AE86-1B4F-A87F-8B26CAC6F657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8FBD77-2194-2A4B-9CDF-23F79939C61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bosses" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2110" uniqueCount="913">
   <si>
     <t>ID</t>
   </si>
@@ -2763,6 +2763,12 @@
   </si>
   <si>
     <t>red</t>
+  </si>
+  <si>
+    <t>bryophyta</t>
+  </si>
+  <si>
+    <t>Bryophyta</t>
   </si>
 </sst>
 </file>
@@ -3084,11 +3090,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1008"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5648,22 +5654,74 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I49" s="2">
+        <v>1</v>
+      </c>
+      <c r="J49" s="2">
+        <v>1</v>
+      </c>
+      <c r="K49" s="2">
+        <v>50</v>
+      </c>
+      <c r="L49" s="2">
+        <v>75</v>
+      </c>
+      <c r="M49" s="2">
+        <v>75</v>
+      </c>
+      <c r="N49" s="2">
+        <v>100</v>
+      </c>
+      <c r="O49" s="2">
+        <v>100</v>
+      </c>
+      <c r="P49" s="2">
+        <v>150</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10965,8 +11023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F960"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="U143" sqref="U143"/>
+    <sheetView topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="I142" sqref="I142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>